<commit_message>
I got the commit to work!
</commit_message>
<xml_diff>
--- a/240529_Doug_UDA_Unit6_Data_Cleaning_Home_Practice_Version.xlsx
+++ b/240529_Doug_UDA_Unit6_Data_Cleaning_Home_Practice_Version.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Douglas McMahon\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\UDA_tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{047A2E5A-08FF-4087-ABC1-74B2D65F5ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0FFA2E-D4C0-461A-8B14-E041CECBF287}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="2" xr2:uid="{97DF4895-1BA4-4DEF-BA56-16CC39697874}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="13155" activeTab="2" xr2:uid="{97DF4895-1BA4-4DEF-BA56-16CC39697874}"/>
   </bookViews>
   <sheets>
     <sheet name="start" sheetId="1" r:id="rId1"/>
@@ -714,10 +714,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="_-[$$-1009]* #,##0.00_-;\-[$$-1009]* #,##0.00_-;_-[$$-1009]* &quot;-&quot;??_-;_-@_-"/>
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-[$$-1009]* #,##0.00_-;\-[$$-1009]* #,##0.00_-;_-[$$-1009]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -743,16 +752,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1071,15 +1083,15 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.68359375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1090,12 +1102,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1109,7 +1121,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1123,7 +1135,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1137,7 +1149,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1151,7 +1163,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1165,7 +1177,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1179,7 +1191,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1193,7 +1205,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1207,7 +1219,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>0</v>
       </c>
@@ -1215,12 +1227,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1234,7 +1246,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1248,7 +1260,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1262,7 +1274,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -1276,7 +1288,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -1290,7 +1302,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -1304,7 +1316,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -1318,7 +1330,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -1332,7 +1344,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -1346,7 +1358,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -1360,7 +1372,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -1374,7 +1386,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -1388,7 +1400,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>81</v>
       </c>
@@ -1402,7 +1414,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>85</v>
       </c>
@@ -1416,7 +1428,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>88</v>
       </c>
@@ -1430,7 +1442,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>92</v>
       </c>
@@ -1444,7 +1456,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>95</v>
       </c>
@@ -1458,7 +1470,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -1472,7 +1484,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>102</v>
       </c>
@@ -1486,7 +1498,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>0</v>
       </c>
@@ -1494,12 +1506,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>106</v>
       </c>
@@ -1513,7 +1525,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>110</v>
       </c>
@@ -1527,7 +1539,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>114</v>
       </c>
@@ -1541,7 +1553,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>118</v>
       </c>
@@ -1555,7 +1567,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>121</v>
       </c>
@@ -1569,7 +1581,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>125</v>
       </c>
@@ -1583,7 +1595,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>129</v>
       </c>
@@ -1597,7 +1609,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>133</v>
       </c>
@@ -1611,7 +1623,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>0</v>
       </c>
@@ -1619,12 +1631,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>138</v>
       </c>
@@ -1638,7 +1650,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>142</v>
       </c>
@@ -1652,7 +1664,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>146</v>
       </c>
@@ -1666,7 +1678,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>0</v>
       </c>
@@ -1674,12 +1686,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>151</v>
       </c>
@@ -1693,7 +1705,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>155</v>
       </c>
@@ -1707,7 +1719,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>159</v>
       </c>
@@ -1721,7 +1733,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>0</v>
       </c>
@@ -1729,12 +1741,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>163</v>
       </c>
@@ -1748,7 +1760,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>167</v>
       </c>
@@ -1762,7 +1774,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>0</v>
       </c>
@@ -1770,12 +1782,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>172</v>
       </c>
@@ -1789,7 +1801,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>176</v>
       </c>
@@ -1803,7 +1815,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>180</v>
       </c>
@@ -1817,7 +1829,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>184</v>
       </c>
@@ -1831,7 +1843,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>0</v>
       </c>
@@ -1839,12 +1851,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>189</v>
       </c>
@@ -1858,7 +1870,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>193</v>
       </c>
@@ -1872,7 +1884,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>197</v>
       </c>
@@ -1886,7 +1898,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>201</v>
       </c>
@@ -1900,7 +1912,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>0</v>
       </c>
@@ -1908,12 +1920,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>206</v>
       </c>
@@ -1927,7 +1939,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>210</v>
       </c>
@@ -1941,7 +1953,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>0</v>
       </c>
@@ -1949,12 +1961,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>215</v>
       </c>
@@ -1968,7 +1980,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>219</v>
       </c>
@@ -1982,7 +1994,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>221</v>
       </c>
@@ -1993,7 +2005,7 @@
         <v>44287</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>222</v>
       </c>
@@ -2018,15 +2030,15 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.68359375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.68359375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.68359375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>223</v>
       </c>
@@ -2040,7 +2052,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -2054,7 +2066,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -2068,7 +2080,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -2082,7 +2094,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2096,7 +2108,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -2110,7 +2122,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -2124,7 +2136,7 @@
         <v>4.45</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -2138,7 +2150,7 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -2152,7 +2164,7 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>33</v>
       </c>
@@ -2166,7 +2178,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>33</v>
       </c>
@@ -2180,7 +2192,7 @@
         <v>2.69</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
@@ -2194,7 +2206,7 @@
         <v>2.92</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
@@ -2208,7 +2220,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>33</v>
       </c>
@@ -2222,7 +2234,7 @@
         <v>12.13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>33</v>
       </c>
@@ -2236,7 +2248,7 @@
         <v>11.67</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>33</v>
       </c>
@@ -2250,7 +2262,7 @@
         <v>15.69</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>33</v>
       </c>
@@ -2264,7 +2276,7 @@
         <v>3.88</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>33</v>
       </c>
@@ -2278,7 +2290,7 @@
         <v>1.46</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>33</v>
       </c>
@@ -2292,7 +2304,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>33</v>
       </c>
@@ -2306,7 +2318,7 @@
         <v>4.8099999999999996</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
@@ -2320,7 +2332,7 @@
         <v>2.48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>33</v>
       </c>
@@ -2334,7 +2346,7 @@
         <v>2.29</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>33</v>
       </c>
@@ -2348,7 +2360,7 @@
         <v>2.48</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>33</v>
       </c>
@@ -2362,7 +2374,7 @@
         <v>1.91</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>33</v>
       </c>
@@ -2376,7 +2388,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>33</v>
       </c>
@@ -2390,7 +2402,7 @@
         <v>3.28</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
@@ -2404,7 +2416,7 @@
         <v>3.47</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>33</v>
       </c>
@@ -2418,7 +2430,7 @@
         <v>13.75</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>105</v>
       </c>
@@ -2432,7 +2444,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>105</v>
       </c>
@@ -2446,7 +2458,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>105</v>
       </c>
@@ -2460,7 +2472,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>105</v>
       </c>
@@ -2474,7 +2486,7 @@
         <v>2.48</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>105</v>
       </c>
@@ -2488,7 +2500,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>105</v>
       </c>
@@ -2502,7 +2514,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>105</v>
       </c>
@@ -2516,7 +2528,7 @@
         <v>28500</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>105</v>
       </c>
@@ -2530,7 +2542,7 @@
         <v>24715.31</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>137</v>
       </c>
@@ -2544,7 +2556,7 @@
         <v>150.55000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>137</v>
       </c>
@@ -2558,7 +2570,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>137</v>
       </c>
@@ -2572,7 +2584,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>150</v>
       </c>
@@ -2586,7 +2598,7 @@
         <v>43.58</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>150</v>
       </c>
@@ -2600,7 +2612,7 @@
         <v>32.86</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>150</v>
       </c>
@@ -2614,7 +2626,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>162</v>
       </c>
@@ -2628,7 +2640,7 @@
         <v>1066.57</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>162</v>
       </c>
@@ -2642,7 +2654,7 @@
         <v>15250</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>171</v>
       </c>
@@ -2656,7 +2668,7 @@
         <v>54.67</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>171</v>
       </c>
@@ -2670,7 +2682,7 @@
         <v>43.75</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>171</v>
       </c>
@@ -2684,7 +2696,7 @@
         <v>99.84</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>171</v>
       </c>
@@ -2698,7 +2710,7 @@
         <v>117.33</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>188</v>
       </c>
@@ -2712,7 +2724,7 @@
         <v>1356.67</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>188</v>
       </c>
@@ -2726,7 +2738,7 @@
         <v>1116.74</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>188</v>
       </c>
@@ -2740,7 +2752,7 @@
         <v>2188.2399999999998</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>188</v>
       </c>
@@ -2754,7 +2766,7 @@
         <v>1770.88</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>205</v>
       </c>
@@ -2768,7 +2780,7 @@
         <v>3761.09</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>205</v>
       </c>
@@ -2782,7 +2794,7 @@
         <v>3292.77</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>214</v>
       </c>
@@ -2807,784 +2819,784 @@
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.68359375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.68359375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.68359375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>223</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="4">
         <v>20</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="4">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="4">
         <v>80</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <v>10.199999999999999</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="4">
         <v>6</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="4">
         <v>7.5</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="4">
         <v>4.54</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4">
         <v>4.45</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="4">
         <v>2.15</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="4">
         <v>2.38</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="4">
         <v>1.89</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="4">
         <v>1.88</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="4">
         <v>2.2400000000000002</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="4">
         <v>2.6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="4">
         <v>2.68</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="4">
         <v>2.69</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="4">
         <v>3.93</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="4">
         <v>2.92</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="4">
         <v>3.67</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="4">
         <v>2.7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="4">
         <v>10.66</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="4">
         <v>12.13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="4">
         <v>12.22</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="4">
         <v>11.67</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="4">
         <v>14.71</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="4">
         <v>15.69</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="4">
         <v>3.93</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="4">
         <v>3.88</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="4">
         <v>1.85</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="4">
         <v>1.46</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="4">
         <v>4.04</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="4">
         <v>3.1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="4">
         <v>3.84</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="4">
         <v>4.8099999999999996</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="4">
         <v>3.72</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="4">
         <v>2.48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="4">
         <v>2.77</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="4">
         <v>2.29</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="4">
         <v>2.4900000000000002</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="4">
         <v>2.48</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="4">
         <v>2.5</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="4">
         <v>1.91</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="4">
         <v>16</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="4">
         <v>3.55</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="4">
         <v>3.28</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="4">
         <v>3.73</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="4">
         <v>3.47</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="4">
         <v>15</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="4">
         <v>13.75</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="4">
         <v>3.5</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="4">
         <v>97.5</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="4">
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="4">
         <v>3.83</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="4">
         <v>1.65</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="4">
         <v>2.48</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="4">
         <v>30</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="4">
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="4">
         <v>0.98</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="4">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="4">
         <v>25000</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="4">
         <v>28500</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="4">
         <v>25246.74</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="4">
         <v>24715.31</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="4">
         <v>224.75</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="4">
         <v>150.55000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="4">
         <v>0.31</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="4">
         <v>0.33</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="4">
         <v>90.19</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="4">
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>150</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="4">
         <v>55.45</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="4">
         <v>43.58</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>150</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="4">
         <v>18.22</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="4">
         <v>32.86</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>150</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="4">
         <v>15</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="4">
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="4">
         <v>1027.8900000000001</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="4">
         <v>1066.57</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="4">
         <v>8892</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="4">
         <v>15250</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>171</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="4">
         <v>65.17</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45" s="4">
         <v>54.67</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>171</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="4">
         <v>45.68</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46" s="4">
         <v>43.75</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>171</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="4">
         <v>107.97</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47" s="4">
         <v>99.84</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>171</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="4">
         <v>125.13</v>
       </c>
-      <c r="D48" s="2">
+      <c r="D48" s="4">
         <v>117.33</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>188</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="4">
         <v>1155.55</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D49" s="4">
         <v>1356.67</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>188</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="4">
         <v>982.28</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D50" s="4">
         <v>1116.74</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>188</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="4">
         <v>1747</v>
       </c>
-      <c r="D51" s="2">
+      <c r="D51" s="4">
         <v>2188.2399999999998</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>188</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="4">
         <v>1505.67</v>
       </c>
-      <c r="D52" s="2">
+      <c r="D52" s="4">
         <v>1770.88</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>205</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="4">
         <v>3560.14</v>
       </c>
-      <c r="D53" s="2">
+      <c r="D53" s="4">
         <v>3761.09</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>205</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="4">
         <v>2553.36</v>
       </c>
-      <c r="D54" s="2">
+      <c r="D54" s="4">
         <v>3292.77</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>214</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="4">
         <v>3969.53</v>
       </c>
-      <c r="D55" s="2">
+      <c r="D55" s="4">
         <v>4045.41</v>
       </c>
     </row>
@@ -3595,6 +3607,29 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaLengthInSeconds xmlns="d1a7958c-8f44-4e0c-83af-8e38a59b607c" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d1a7958c-8f44-4e0c-83af-8e38a59b607c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="5aac8420-433a-44e6-985a-8fb3279679a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EF2CCE6057B15645B7106B4D97933848" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bf5962951a358addb2c8c1b30087ca4d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="d1a7958c-8f44-4e0c-83af-8e38a59b607c" xmlns:ns3="5aac8420-433a-44e6-985a-8fb3279679a5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e87beb4acede310079b2dfa005ce1c0d" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3846,30 +3881,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaLengthInSeconds xmlns="d1a7958c-8f44-4e0c-83af-8e38a59b607c" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d1a7958c-8f44-4e0c-83af-8e38a59b607c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="5aac8420-433a-44e6-985a-8fb3279679a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32F5D4B0-F782-4D01-99D7-460B43E817A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68B6B941-2580-427B-AC20-DB2B52A0634A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="d1a7958c-8f44-4e0c-83af-8e38a59b607c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="5aac8420-433a-44e6-985a-8fb3279679a5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{585B0249-FE96-4001-B7B7-B4439DDA63E8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3887,24 +3925,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68B6B941-2580-427B-AC20-DB2B52A0634A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d1a7958c-8f44-4e0c-83af-8e38a59b607c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="5aac8420-433a-44e6-985a-8fb3279679a5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32F5D4B0-F782-4D01-99D7-460B43E817A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>